<commit_message>
added date functionality for easy identification
</commit_message>
<xml_diff>
--- a/HouseChores/2HouseChores.xlsx
+++ b/HouseChores/2HouseChores.xlsx
@@ -16,11 +16,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>HOUSE CHORES</t>
   </si>
   <si>
+    <t>Dated 18-Nov-2018 to 25-Nov-2018</t>
+  </si>
+  <si>
     <t>Day</t>
   </si>
   <si>
@@ -51,13 +54,13 @@
     <t>Harry</t>
   </si>
   <si>
+    <t>Mwai</t>
+  </si>
+  <si>
+    <t>dan</t>
+  </si>
+  <si>
     <t>Marvinus</t>
-  </si>
-  <si>
-    <t>dan</t>
-  </si>
-  <si>
-    <t>Mwai</t>
   </si>
   <si>
     <t>Tuesday</t>
@@ -212,7 +215,7 @@
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="3" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -243,7 +246,7 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="3" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -798,18 +801,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D13" activeCellId="0" pane="topLeft" sqref="D13"/>
+      <selection activeCell="K3" activeCellId="0" pane="topLeft" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="11" width="8.94"/>
     <col customWidth="1" max="2" min="2" style="11" width="6.98"/>
-    <col customWidth="1" max="3" min="3" style="11" width="8.85"/>
-    <col customWidth="1" max="4" min="4" style="11" width="8.85"/>
+    <col customWidth="1" max="4" min="3" style="11" width="8.85"/>
     <col customWidth="1" max="5" min="5" style="11" width="15.35"/>
     <col customWidth="1" max="6" min="6" style="11" width="6.98"/>
     <col customWidth="1" max="8" min="7" style="11" width="8.85"/>
@@ -822,81 +824,58 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="14" spans="1:10">
-      <c r="A2" s="16" t="s">
+    <row customHeight="1" ht="22.05" r="2" s="14" spans="1:10">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+    </row>
+    <row customHeight="1" ht="15" r="3" s="14" spans="1:10">
+      <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="D3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="F3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="G3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="11" t="n"/>
-      <c r="J2" s="11" t="n"/>
-    </row>
-    <row customHeight="1" ht="13.8" r="3" s="14" spans="1:10">
-      <c r="A3" s="18" t="n"/>
-      <c r="B3" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="18" t="n"/>
-      <c r="E3" s="18" t="n"/>
-      <c r="F3" s="18" t="n"/>
-      <c r="G3" s="18" t="n"/>
-      <c r="H3" s="18" t="n"/>
+      <c r="H3" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="I3" s="11" t="n"/>
       <c r="J3" s="11" t="n"/>
     </row>
     <row customHeight="1" ht="13.8" r="4" s="14" spans="1:10">
-      <c r="A4" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>13</v>
-      </c>
+      <c r="A4" s="18" t="n"/>
+      <c r="B4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="18" t="n"/>
+      <c r="E4" s="18" t="n"/>
+      <c r="F4" s="18" t="n"/>
+      <c r="G4" s="18" t="n"/>
+      <c r="H4" s="18" t="n"/>
       <c r="I4" s="11" t="n"/>
       <c r="J4" s="11" t="n"/>
     </row>
     <row customHeight="1" ht="13.8" r="5" s="14" spans="1:10">
       <c r="A5" s="18" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>11</v>
@@ -905,42 +884,44 @@
         <v>12</v>
       </c>
       <c r="E5" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>15</v>
-      </c>
       <c r="G5" s="18" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>10</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="I5" s="11" t="n"/>
+      <c r="J5" s="11" t="n"/>
     </row>
     <row customHeight="1" ht="13.8" r="6" s="14" spans="1:10">
       <c r="A6" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="7" s="14" spans="1:10">
@@ -948,51 +929,51 @@
         <v>17</v>
       </c>
       <c r="B7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>15</v>
-      </c>
       <c r="G7" s="18" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="8" s="14" spans="1:10">
       <c r="A8" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="9" s="14" spans="1:10">
@@ -1000,25 +981,25 @@
         <v>20</v>
       </c>
       <c r="B9" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>15</v>
-      </c>
       <c r="G9" s="18" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="10" s="14" spans="1:10">
@@ -1026,31 +1007,58 @@
         <v>21</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="11" s="14" spans="1:10">
+      <c r="A11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="C11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>12</v>
+      <c r="F11" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>

</xml_diff>